<commit_message>
spreadsheets_v2: test more types
</commit_message>
<xml_diff>
--- a/corehq/util/spreadsheets_v2/tests/files/xlsx/types.xlsx
+++ b/corehq/util/spreadsheets_v2/tests/files/xlsx/types.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,25 +27,52 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Date of Birth</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Danny</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>Float</t>
+  </si>
+  <si>
+    <t>Bool-T</t>
+  </si>
+  <si>
+    <t>Bool-F</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>Int.0</t>
+  </si>
+  <si>
+    <t>Calculation</t>
+  </si>
+  <si>
+    <t>Styled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -53,13 +80,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -71,14 +117,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Accent4" xfId="1" builtinId="41"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -354,39 +406,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>32331</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add max_row to spreadsheets_v2.Worksheet
</commit_message>
<xml_diff>
--- a/corehq/util/spreadsheets_v2/tests/files/xlsx/types.xlsx
+++ b/corehq/util/spreadsheets_v2/tests/files/xlsx/types.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Danny</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Styled</t>
+  </si>
+  <si>
+    <t>Empty Date</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,6 +503,12 @@
         <v>11</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix and test spreadsheet_v2 date/time correctness issues
</commit_message>
<xml_diff>
--- a/corehq/util/spreadsheets_v2/tests/files/xlsx/types.xlsx
+++ b/corehq/util/spreadsheets_v2/tests/files/xlsx/types.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Danny</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>Empty Date</t>
+  </si>
+  <si>
+    <t>Date Time</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Midnight</t>
   </si>
 </sst>
 </file>
@@ -124,13 +133,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent4" xfId="1" builtinId="41"/>
@@ -409,13 +420,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -435,79 +449,103 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="B3" s="6">
+        <v>42370.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>5.0999999999999996</v>
+        <v>15</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="b">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
         <v>5</v>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.49</v>
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B13">
         <f>1+1</f>
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>